<commit_message>
Ajout hyp + état 5 + massflow
</commit_message>
<xml_diff>
--- a/Param/Projet_contraintes.xlsx
+++ b/Param/Projet_contraintes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julem\Dropbox\EPL\Master_1\Q1\LELME2150 Thermal Cycles\2024\Projet\Param\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/louisevaessen/Documents/Thermal_Project/Param/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946C17EF-FF05-408A-AA44-3EEEF5274CC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA477D26-DEEB-FE49-9DF0-3476F6E56640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11715" yWindow="615" windowWidth="21600" windowHeight="11385" xr2:uid="{CB6374FC-8A30-4020-B8B5-DB38D12B49A4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{CB6374FC-8A30-4020-B8B5-DB38D12B49A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -23,12 +23,8 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
   <si>
     <t>T_max</t>
   </si>
@@ -143,13 +139,22 @@
     <t>T_pinch_evap_I</t>
   </si>
   <si>
-    <t>diofférence T entre sortie de l'evaporateur I et etat 1</t>
-  </si>
-  <si>
     <t>T_hot_fluid_in_II</t>
   </si>
   <si>
     <t>p_hot_fluid</t>
+  </si>
+  <si>
+    <t>T_cd_subcool</t>
+  </si>
+  <si>
+    <t>différence T entre sortie de l'evaporateur I et etat 1</t>
+  </si>
+  <si>
+    <t>Limite technologique de la turbine</t>
+  </si>
+  <si>
+    <t>p_3</t>
   </si>
 </sst>
 </file>
@@ -586,17 +591,17 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="49.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="49.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -619,7 +624,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -633,7 +638,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -653,7 +658,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -667,7 +672,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -681,7 +686,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -692,7 +697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -703,7 +708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -717,7 +722,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -731,7 +736,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -745,7 +750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -760,7 +765,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -774,7 +779,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -788,13 +793,13 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>17</v>
       </c>
       <c r="B14">
-        <f>273.15+10</f>
-        <v>283.14999999999998</v>
+        <f>273.15+8</f>
+        <v>281.14999999999998</v>
       </c>
       <c r="C14" t="s">
         <v>20</v>
@@ -803,13 +808,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>18</v>
       </c>
       <c r="B15">
-        <f>273.15+20</f>
-        <v>293.14999999999998</v>
+        <f>273.15+28</f>
+        <v>301.14999999999998</v>
       </c>
       <c r="C15" t="s">
         <v>20</v>
@@ -818,9 +823,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16">
         <f>140+273.15</f>
@@ -833,13 +838,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>0</v>
       </c>
       <c r="B17">
-        <f>140+273.15</f>
-        <v>413.15</v>
+        <f>838.15</f>
+        <v>838.15</v>
       </c>
       <c r="C17" t="s">
         <v>20</v>
@@ -847,8 +852,11 @@
       <c r="D17" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -859,10 +867,10 @@
         <v>0</v>
       </c>
       <c r="F18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -876,73 +884,104 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20">
         <v>1000000</v>
       </c>
+      <c r="C20" t="s">
+        <v>8</v>
+      </c>
       <c r="D20" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>20</v>
+      </c>
       <c r="D21" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22">
+        <f>310*10^5</f>
+        <v>31000000</v>
+      </c>
+      <c r="C22" t="s">
+        <v>8</v>
+      </c>
       <c r="D22" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D23" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D24" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D25" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D26" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D27" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D28" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D29" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D30" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D31" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D32" s="2" t="b">
         <v>0</v>
       </c>

</xml_diff>